<commit_message>
Scriptie - experimentgrafieken geupdate
</commit_message>
<xml_diff>
--- a/Ploegen berekening TN feb.xlsx
+++ b/Ploegen berekening TN feb.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Kg totaal matrix</t>
   </si>
@@ -264,10 +264,13 @@
     <t>AVG(AVG(LijnSnelheid)) (stuks/min)</t>
   </si>
   <si>
-    <t>AVG(AVG(OEE)) (fractal (0-1))</t>
-  </si>
-  <si>
-    <t>AVG(Ploegen na)</t>
+    <t>Gem. ploegen na ovens</t>
+  </si>
+  <si>
+    <t>Gem. ploegen voor ovens</t>
+  </si>
+  <si>
+    <t>Gem. ploegen voor persen</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -387,6 +390,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Procent" xfId="1" builtinId="5"/>
@@ -425,7 +429,7 @@
         <xdr:cNvPr id="2" name="Equals 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -769,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -779,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="M71" sqref="M71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +802,7 @@
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1022,6 +1026,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D20" s="15" t="s">
         <v>75</v>
@@ -1029,6 +1041,14 @@
       <c r="E20" s="15" t="s">
         <v>76</v>
       </c>
+      <c r="M20" s="9">
+        <f>AVERAGE(M25:M41)</f>
+        <v>4.3520906901170848</v>
+      </c>
+      <c r="N20" s="9">
+        <f>AVERAGE(N25:N41)</f>
+        <v>8.44344574023498E-3</v>
+      </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
@@ -1042,13 +1062,16 @@
         <v>95907961</v>
       </c>
       <c r="E21">
-        <v>88181000</v>
+        <v>88214000</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -1058,14 +1081,18 @@
       </c>
       <c r="E22">
         <f>E21/D21*D22</f>
-        <v>91.943358070139766</v>
+        <v>91.977766058440139</v>
       </c>
       <c r="F22" t="s">
         <v>77</v>
       </c>
       <c r="M22" s="9">
-        <f>AVERAGE(M25:M41)</f>
-        <v>4.0433706699256398</v>
+        <f>AVERAGE(M66:M68)</f>
+        <v>2.3239866524909697E-2</v>
+      </c>
+      <c r="N22" s="9">
+        <f>AVERAGE(N66:N68)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1107,7 +1134,7 @@
         <v>5762552</v>
       </c>
       <c r="F25">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="G25">
         <v>1000</v>
@@ -1124,7 +1151,7 @@
       </c>
       <c r="M25" s="9">
         <f t="shared" ref="M25:M41" si="0">F25*H25/(J25*H25*480*L25)</f>
-        <v>9.3471136663787879E-3</v>
+        <v>0.18694227332757574</v>
       </c>
       <c r="N25" s="9">
         <f>G25*H25/(J25*H25*480*L25)</f>
@@ -1171,7 +1198,7 @@
         <v>8029520</v>
       </c>
       <c r="F27">
-        <v>2590000</v>
+        <v>2699000</v>
       </c>
       <c r="G27">
         <v>1000</v>
@@ -1188,7 +1215,7 @@
       </c>
       <c r="M27" s="9">
         <f t="shared" si="0"/>
-        <v>18.407742262781756</v>
+        <v>19.182431029825466</v>
       </c>
       <c r="N27" s="9">
         <f t="shared" si="1"/>
@@ -1203,10 +1230,10 @@
         <v>9788896</v>
       </c>
       <c r="F28">
-        <v>2653000</v>
+        <v>2518000</v>
       </c>
       <c r="G28">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="H28" s="20">
         <f>3.47811007659957/1000</f>
@@ -1220,11 +1247,11 @@
       </c>
       <c r="M28" s="9">
         <f>F28*H28/(J28*H28*480*L28)</f>
-        <v>15.65852954391791</v>
+        <v>14.861732902972218</v>
       </c>
       <c r="N28" s="9">
         <f>G28*H28/(J28*H28*480*L28)</f>
-        <v>2.3608789361353803E-2</v>
+        <v>5.9021973403384506E-3</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
@@ -1235,7 +1262,7 @@
         <v>7846772</v>
       </c>
       <c r="F29">
-        <v>40000</v>
+        <v>76000</v>
       </c>
       <c r="G29">
         <v>1000</v>
@@ -1252,7 +1279,7 @@
       </c>
       <c r="M29" s="9">
         <f t="shared" si="0"/>
-        <v>0.31419735807327243</v>
+        <v>0.59697498033921759</v>
       </c>
       <c r="N29" s="9">
         <f t="shared" si="1"/>
@@ -1299,7 +1326,7 @@
         <v>3501620</v>
       </c>
       <c r="F31">
-        <v>29000</v>
+        <v>76000</v>
       </c>
       <c r="G31">
         <v>1000</v>
@@ -1316,7 +1343,7 @@
       </c>
       <c r="M31" s="9">
         <f t="shared" si="0"/>
-        <v>0.55228859289172139</v>
+        <v>1.4473770020610628</v>
       </c>
       <c r="N31" s="9">
         <f t="shared" si="1"/>
@@ -1427,7 +1454,7 @@
         <v>12187040</v>
       </c>
       <c r="F35">
-        <v>2181000</v>
+        <v>2523000</v>
       </c>
       <c r="G35">
         <v>1000</v>
@@ -1444,7 +1471,7 @@
       </c>
       <c r="M35" s="9">
         <f t="shared" si="0"/>
-        <v>9.9880773427401337</v>
+        <v>11.554295798135424</v>
       </c>
       <c r="N35" s="9">
         <f t="shared" si="1"/>
@@ -1459,7 +1486,7 @@
         <v>12407600</v>
       </c>
       <c r="F36">
-        <v>2318000</v>
+        <v>2528000</v>
       </c>
       <c r="G36">
         <v>1000</v>
@@ -1476,7 +1503,7 @@
       </c>
       <c r="M36" s="9">
         <f t="shared" si="0"/>
-        <v>10.494524151743196</v>
+        <v>11.445279143920104</v>
       </c>
       <c r="N36" s="9">
         <f t="shared" si="1"/>
@@ -1491,7 +1518,7 @@
         <v>15327560</v>
       </c>
       <c r="F37">
-        <v>55000</v>
+        <v>1000</v>
       </c>
       <c r="G37">
         <v>1000</v>
@@ -1508,7 +1535,7 @@
       </c>
       <c r="M37" s="9">
         <f t="shared" si="0"/>
-        <v>0.21979095424129719</v>
+        <v>3.9961991680235853E-3</v>
       </c>
       <c r="N37" s="9">
         <f t="shared" si="1"/>
@@ -1587,7 +1614,7 @@
         <v>12088104</v>
       </c>
       <c r="F40">
-        <v>2507000</v>
+        <v>2762000</v>
       </c>
       <c r="G40">
         <v>1000</v>
@@ -1604,7 +1631,7 @@
       </c>
       <c r="M40" s="9">
         <f t="shared" si="0"/>
-        <v>13.01681678529294</v>
+        <v>14.34082487474236</v>
       </c>
       <c r="N40" s="9">
         <f t="shared" si="1"/>
@@ -1619,7 +1646,7 @@
         <v>10638560</v>
       </c>
       <c r="F41">
-        <v>1000</v>
+        <v>47000</v>
       </c>
       <c r="G41">
         <v>1000</v>
@@ -1636,7 +1663,7 @@
       </c>
       <c r="M41" s="9">
         <f t="shared" si="0"/>
-        <v>6.2978313937329848E-3</v>
+        <v>0.29599807550545032</v>
       </c>
       <c r="N41" s="9">
         <f>G41*H41/(J41*H41*480*L41)</f>
@@ -2132,7 +2159,7 @@
         <v>34246634.877882801</v>
       </c>
       <c r="F66">
-        <v>6100000</v>
+        <v>5871000</v>
       </c>
       <c r="H66" s="20">
         <f>3.35756802558899/1000</f>
@@ -2147,9 +2174,12 @@
       </c>
       <c r="M66" s="9">
         <f>F66*H66/(J66*H66*480*L66)</f>
-        <v>2.8108645046153145E-2</v>
-      </c>
-      <c r="N66" s="9"/>
+        <v>2.705341886327297E-2</v>
+      </c>
+      <c r="N66" s="9">
+        <f>G66*H66/(J66*H66*480*L66)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
@@ -2160,7 +2190,7 @@
         <v>1711510.3729148097</v>
       </c>
       <c r="F67">
-        <v>57000</v>
+        <v>76000</v>
       </c>
       <c r="H67" s="20">
         <f>52.9669226284685/1000</f>
@@ -2175,9 +2205,12 @@
       </c>
       <c r="M67" s="9">
         <f>F67*H67/(J67*H67*480*L67)</f>
-        <v>5.0637934803451114E-3</v>
-      </c>
-      <c r="N67" s="9"/>
+        <v>6.7517246404601482E-3</v>
+      </c>
+      <c r="N67" s="9">
+        <f t="shared" ref="N67:N68" si="2">G67*H67/(J67*H67*480*L67)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
@@ -2188,7 +2221,7 @@
         <v>31899571.911138851</v>
       </c>
       <c r="F68">
-        <v>7259000</v>
+        <v>7523000</v>
       </c>
       <c r="H68" s="20">
         <f>3.38800001144409/1000</f>
@@ -2203,9 +2236,12 @@
       </c>
       <c r="M68" s="9">
         <f>F68*H68/(J68*H68*480*L68)</f>
-        <v>3.4654132210469181E-2</v>
-      </c>
-      <c r="N68" s="9"/>
+        <v>3.5914456070995963E-2</v>
+      </c>
+      <c r="N68" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H70" s="15" t="s">
@@ -2214,12 +2250,8 @@
       <c r="J70" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="L70" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="M70" s="15" t="s">
-        <v>82</v>
-      </c>
+      <c r="L70" s="26"/>
+      <c r="M70" s="26"/>
     </row>
     <row r="71" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F71">

</xml_diff>

<commit_message>
Scriptie - Eindconclusie aangepast na feedback van Frank
</commit_message>
<xml_diff>
--- a/Ploegen berekening TN feb.xlsx
+++ b/Ploegen berekening TN feb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="25200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
         <xdr:cNvPr id="2" name="Equals 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{81193C8A-C1C1-4CDE-AFB3-EDEEA4AEF6F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -773,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -781,9 +781,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
       <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
@@ -2274,6 +2274,12 @@
     </row>
     <row r="72" spans="4:14" x14ac:dyDescent="0.25">
       <c r="M72" s="18"/>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J73" s="19"/>
+    </row>
+    <row r="74" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J74" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>